<commit_message>
Update mkr_names for use with markers_all file
</commit_message>
<xml_diff>
--- a/mkr_names.xlsx
+++ b/mkr_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a724e9db8ad8f00/Erasmus MC Neuroscience/Code/OpenSim-Santos2017-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC104867219E66FE5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E791BE28-6A57-4C71-BA12-E7864DF6FEF5}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_F25DC773A252ABDACC104867219E66FE5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B450EED3-0E6D-46AC-A4ED-EDBAC1EEFE10}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
   <si>
     <t>Rajagopal 2015</t>
   </si>
@@ -370,6 +370,24 @@
   </si>
   <si>
     <t>LGTRO</t>
+  </si>
+  <si>
+    <t>RMT2</t>
+  </si>
+  <si>
+    <t>LMT2</t>
+  </si>
+  <si>
+    <t>RTTC</t>
+  </si>
+  <si>
+    <t>LTTC</t>
+  </si>
+  <si>
+    <t>RFAX</t>
+  </si>
+  <si>
+    <t>LFAX</t>
   </si>
 </sst>
 </file>
@@ -687,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,484 +752,536 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>71</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>72</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>73</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>85</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>86</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B50" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>88</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>89</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B53" t="s">
         <v>38</v>
       </c>
-      <c r="C47" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>94</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B59" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>95</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>100</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B65" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>101</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B66" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>103</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B68" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>104</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B69" t="s">
         <v>41</v>
       </c>
-      <c r="C62" t="s">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>105</v>
-      </c>
-      <c r="B63" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>110</v>
       </c>
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>111</v>
       </c>
-      <c r="C69" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>112</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B78" t="s">
         <v>15</v>
       </c>
-      <c r="C70" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>113</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B79" t="s">
         <v>22</v>
       </c>
-      <c r="C71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>114</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B80" t="s">
         <v>23</v>
       </c>
-      <c r="C72" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>119</v>
+      </c>
+      <c r="B81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>120</v>
+      </c>
+      <c r="B82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>117</v>
+      </c>
+      <c r="B83" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>118</v>
+      </c>
+      <c r="B84" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>